<commit_message>
Deprecate license guessing (stage 2)
</commit_message>
<xml_diff>
--- a/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B43F4-6420-4D77-9BAE-981EA2068EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0EAEA-79FC-4317-ACB6-B04A3E8D88B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,18 +245,6 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
-  </si>
-  <si>
-    <t>Guessed License URL</t>
-  </si>
-  <si>
-    <t>Guessed License URL AuditInfo</t>
-  </si>
-  <si>
-    <t>$guessedLicenseUrl$</t>
-  </si>
-  <si>
-    <t>$guessedLicenseUrlAuditInfo$</t>
   </si>
 </sst>
 </file>
@@ -295,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,18 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -444,8 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,18 +706,18 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="25.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.15234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.53515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.15234375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.15234375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -751,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
@@ -759,8 +733,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
@@ -774,7 +748,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -788,7 +762,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -802,7 +776,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -816,7 +790,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -836,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -856,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -869,35 +843,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.69140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.15234375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.54296875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.1796875" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.7265625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.54296875" style="6" customWidth="1"/>
-    <col min="14" max="15" width="31.54296875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="20.453125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="20.1796875" style="7" customWidth="1"/>
-    <col min="18" max="18" width="29.54296875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="17.7265625" style="8" customWidth="1"/>
-    <col min="20" max="20" width="19.54296875" style="8" customWidth="1"/>
-    <col min="21" max="21" width="19.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.69140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.4609375" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.53515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.15234375" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.69140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.53515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.4609375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.15234375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="29.53515625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.69140625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="19.53515625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="19.53515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -937,32 +910,26 @@
       <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1002,28 +969,22 @@
       <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deprecate license guessing (stage 2) (#318)
</commit_message>
<xml_diff>
--- a/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B43F4-6420-4D77-9BAE-981EA2068EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0EAEA-79FC-4317-ACB6-B04A3E8D88B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,18 +245,6 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
-  </si>
-  <si>
-    <t>Guessed License URL</t>
-  </si>
-  <si>
-    <t>Guessed License URL AuditInfo</t>
-  </si>
-  <si>
-    <t>$guessedLicenseUrl$</t>
-  </si>
-  <si>
-    <t>$guessedLicenseUrlAuditInfo$</t>
   </si>
 </sst>
 </file>
@@ -295,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,18 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -444,8 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,18 +706,18 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="25.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.15234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.53515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.15234375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.15234375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -751,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
@@ -759,8 +733,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
@@ -774,7 +748,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -788,7 +762,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -802,7 +776,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -816,7 +790,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -836,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -856,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -869,35 +843,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.69140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.15234375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.54296875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.1796875" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.7265625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.54296875" style="6" customWidth="1"/>
-    <col min="14" max="15" width="31.54296875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="20.453125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="20.1796875" style="7" customWidth="1"/>
-    <col min="18" max="18" width="29.54296875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="17.7265625" style="8" customWidth="1"/>
-    <col min="20" max="20" width="19.54296875" style="8" customWidth="1"/>
-    <col min="21" max="21" width="19.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.69140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.4609375" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.53515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.15234375" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.69140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.53515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.4609375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.15234375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="29.53515625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.69140625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="19.53515625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="19.53515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -937,32 +910,26 @@
       <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1002,28 +969,22 @@
       <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add PackageUrl as column to OSS-Inventory
</commit_message>
<xml_diff>
--- a/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0EAEA-79FC-4317-ACB6-B04A3E8D88B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59837DAF-70D6-44B2-AD5C-10D474EF2299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
+  </si>
+  <si>
+    <t>$packageUrl$</t>
+  </si>
+  <si>
+    <t>PackageUrl</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -857,20 +863,20 @@
     <col min="4" max="4" width="11.69140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
     <col min="6" max="6" width="24.69140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.4609375" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.53515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.15234375" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.69140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.53515625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.4609375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="20.15234375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.53515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="17.69140625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="19.53515625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="19.53515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.4609375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="18.53515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.15234375" style="5" customWidth="1"/>
+    <col min="12" max="13" width="28.69140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="31.53515625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.4609375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="20.15234375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="29.53515625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="17.69140625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="19.53515625" style="8" customWidth="1"/>
+    <col min="20" max="20" width="19.53515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -892,44 +898,47 @@
       <c r="G1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -951,40 +960,43 @@
       <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -992,4 +1004,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e760c494-6550-44b4-8258-77c175d778b7}" enabled="1" method="Privileged" siteId="{76a2ae5a-9f00-4f6b-95ed-5d33d77c4d61}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add PackageUrl as column to OSS-Inventory (#330)
</commit_message>
<xml_diff>
--- a/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/core/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0EAEA-79FC-4317-ACB6-B04A3E8D88B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59837DAF-70D6-44B2-AD5C-10D474EF2299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
+  </si>
+  <si>
+    <t>$packageUrl$</t>
+  </si>
+  <si>
+    <t>PackageUrl</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -857,20 +863,20 @@
     <col min="4" max="4" width="11.69140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
     <col min="6" max="6" width="24.69140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.4609375" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.53515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.15234375" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.69140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.53515625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.4609375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="20.15234375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.53515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="17.69140625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="19.53515625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="19.53515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.4609375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="18.53515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.15234375" style="5" customWidth="1"/>
+    <col min="12" max="13" width="28.69140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="31.53515625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="20.4609375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="20.15234375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="29.53515625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="17.69140625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="19.53515625" style="8" customWidth="1"/>
+    <col min="20" max="20" width="19.53515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="9" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -892,44 +898,47 @@
       <c r="G1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -951,40 +960,43 @@
       <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -992,4 +1004,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e760c494-6550-44b4-8258-77c175d778b7}" enabled="1" method="Privileged" siteId="{76a2ae5a-9f00-4f6b-95ed-5d33d77c4d61}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>